<commit_message>
finished draft for GCR
</commit_message>
<xml_diff>
--- a/word/Table3.xlsx
+++ b/word/Table3.xlsx
@@ -523,7 +523,7 @@
   <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F1"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -823,7 +823,7 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+      <c r="A17" s="4" t="s">
         <v>22</v>
       </c>
       <c r="B17" s="7"/>

</xml_diff>